<commit_message>
[add] selectorError, not colored warning
</commit_message>
<xml_diff>
--- a/sample/data.xlsx
+++ b/sample/data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <r>
       <rPr>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t xml:space="preserve">branch_PAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB(255,0,0,2)</t>
   </si>
   <si>
     <t xml:space="preserve">20per</t>
@@ -770,11 +773,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.1777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="81.237037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,9 +947,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,13 +1167,13 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,9 +1181,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,34 +1198,35 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[add] not defined exception
</commit_message>
<xml_diff>
--- a/sample/data.xlsx
+++ b/sample/data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -626,9 +626,6 @@
     <t xml:space="preserve">branch_PAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">RGB(255,0,0,2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">20per</t>
   </si>
   <si>
@@ -638,7 +635,7 @@
     <t xml:space="preserve">ALL()</t>
   </si>
   <si>
-    <t xml:space="preserve">Cool(0,10)</t>
+    <t xml:space="preserve">cool(0,10)</t>
   </si>
   <si>
     <t xml:space="preserve">TOP(1)</t>
@@ -773,11 +770,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="81.237037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="83.2962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,9 +944,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,13 +1164,13 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,7 +1180,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,12 +1195,12 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1211,22 +1208,22 @@
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>